<commit_message>
Slight changes to presentation of data
</commit_message>
<xml_diff>
--- a/src/opt/test/data/COMPARISONS-RO.xlsx
+++ b/src/opt/test/data/COMPARISONS-RO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorit\Documents\spring2019\cs4641\Randomized Optimization\ABAGAIL\src\opt\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABBBCF1-0940-442B-AC2D-3E3D6B643087}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24A390C-C616-4C54-B368-6C99A54AF8D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5DFCDBE1-E3A1-47CA-9768-A11705BAE005}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{5DFCDBE1-E3A1-47CA-9768-A11705BAE005}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Randomized Optimization Training times</t>
   </si>
@@ -53,13 +53,7 @@
     <t>Flip Flop</t>
   </si>
   <si>
-    <t>Map k-Coloring</t>
-  </si>
-  <si>
     <t>MIMIC</t>
-  </si>
-  <si>
-    <t>Time of first iteration</t>
   </si>
   <si>
     <t>N/A</t>
@@ -79,15 +73,28 @@
   <si>
     <t>RHC Error</t>
   </si>
+  <si>
+    <t>Time to Reach Convergence</t>
+  </si>
+  <si>
+    <t>Max k-Coloring</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -109,18 +116,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -21654,7 +21731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C8CB9A-17A9-47BC-B6E4-DFFF363F92EB}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -21662,16 +21739,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -35682,9 +35759,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387EE4A1-549D-44A0-A282-01332E083DEE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
@@ -35693,86 +35770,165 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>359100</v>
-      </c>
-      <c r="C3" s="2">
-        <v>49300</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3595100</v>
-      </c>
-      <c r="E3" s="2">
-        <v>35852000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>13702600</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1307700</v>
+      </c>
+      <c r="D3" s="3">
+        <v>151992700</v>
+      </c>
+      <c r="E3" s="3">
+        <v>14431833400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>109200</v>
-      </c>
-      <c r="C4" s="2">
-        <v>57200</v>
-      </c>
-      <c r="D4" s="2">
-        <v>7586000</v>
-      </c>
-      <c r="E4" s="2">
-        <v>12388700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <v>5534900</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3605500</v>
+      </c>
+      <c r="D4" s="3">
+        <v>347107500</v>
+      </c>
+      <c r="E4" s="3">
+        <v>449707800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10791200</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20257300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
-        <v>650800</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2161600</v>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>13702600</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1307700</v>
+      </c>
+      <c r="D9" s="3">
+        <v>151992700</v>
+      </c>
+      <c r="E9" s="3">
+        <v>14431833400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5534900</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3605500</v>
+      </c>
+      <c r="D10" s="3">
+        <v>347107500</v>
+      </c>
+      <c r="E10" s="3">
+        <v>449707800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10791200</v>
+      </c>
+      <c r="E11" s="3">
+        <v>20257300</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>